<commit_message>
versie v12.7.7 - finaal
</commit_message>
<xml_diff>
--- a/graphics/vergelijking_recon_automatisch.xlsx
+++ b/graphics/vergelijking_recon_automatisch.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{724C1790-C3A8-4367-B425-6ECE3E1E18C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A423B39-BE7B-4FE4-BA01-E529AD30ED83}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3984AAF0-BB45-464A-8B81-864738E25F8B}"/>
+    <workbookView xWindow="4392" yWindow="6876" windowWidth="17280" windowHeight="8880" xr2:uid="{3984AAF0-BB45-464A-8B81-864738E25F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95E40B2-35C5-4B54-8C03-8DB9BB84AC4F}">
   <dimension ref="A2:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>